<commit_message>
new fits and feature importance
</commit_message>
<xml_diff>
--- a/Output/Classifier Fitting/Random Forest/All_Data Training Statistics.xlsx
+++ b/Output/Classifier Fitting/Random Forest/All_Data Training Statistics.xlsx
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>267.4868530035019</v>
+        <v>199.7719016393026</v>
       </c>
       <c r="C2" t="n">
-        <v>0.04455886273588237</v>
+        <v>0.03327867760108322</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.861068276436303</v>
+        <v>0.8615681376630585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>